<commit_message>
loop over values and convert to csv file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luis.g.carlin/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luis.g.carlin/git/parse-spike/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA2EE74F-2BF3-9F41-BCD2-929E482C99AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE58DDDD-B9DA-A34B-8D9E-47772E29F87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{3F44BDD0-2C85-B745-9C62-C8B003794E6B}"/>
   </bookViews>
@@ -31,22 +31,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Luis </t>
+  </si>
+  <si>
+    <t>Carlos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,9 +78,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA5F3F8-2A76-584A-8CF2-BED5BED4B83D}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -405,6 +415,17 @@
         <v>0.6</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>456</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>